<commit_message>
Fix Integer and Numeric
</commit_message>
<xml_diff>
--- a/doc/LoadOuts.xlsx
+++ b/doc/LoadOuts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="15090" windowHeight="12240"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="15090" windowHeight="10335"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -722,7 +722,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
       <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>

</xml_diff>